<commit_message>
trayectory starts from home position
</commit_message>
<xml_diff>
--- a/data Motores.xlsx
+++ b/data Motores.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juans\Desktop\Mecatronica 2021-1\Servos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juans\Desktop\Mecatronica 2020-2\Diseño\Matlab\servos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -384,7 +384,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,5 +517,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>